<commit_message>
Added A List Apart, Bootstrap, Smashing Magazine and Squarespace
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="20580" yWindow="1540" windowWidth="12820" windowHeight="18380" tabRatio="500"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
   <si>
     <t>Twitter</t>
   </si>
@@ -586,6 +586,21 @@
   </si>
   <si>
     <t>FB502B</t>
+  </si>
+  <si>
+    <t>Smashing Magazine</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>Square Space</t>
+  </si>
+  <si>
+    <t>A List Apart</t>
+  </si>
+  <si>
+    <t>E95C33</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1144,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1270,10 +1285,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="C7">
         <v>217</v>
@@ -1283,18 +1298,18 @@
         <v>317</v>
       </c>
       <c r="E7">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F7">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="C8">
         <v>217</v>
@@ -1304,10 +1319,10 @@
         <v>317</v>
       </c>
       <c r="E8">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="F8">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1732,7 +1747,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B29" t="s">
         <v>101</v>
@@ -1753,44 +1768,44 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="C30">
-        <v>199.8</v>
+        <v>200</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>299.8</v>
+        <v>300</v>
       </c>
       <c r="E30">
-        <v>74.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="F30">
-        <v>87.8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>199</v>
+        <v>199.8</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
-        <v>299</v>
+        <v>299.8</v>
       </c>
       <c r="E31">
-        <v>79</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="F31">
-        <v>61</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1816,23 +1831,23 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D33">
         <f>MOD((C33+100),360)</f>
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E33">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F33">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1858,94 +1873,94 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C35">
-        <v>196.9</v>
+        <v>198</v>
       </c>
       <c r="D35">
         <f>MOD((C35+100),360)</f>
-        <v>296.89999999999998</v>
+        <v>298</v>
       </c>
       <c r="E35">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F35">
-        <v>69.400000000000006</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C36">
-        <v>196.3</v>
+        <v>196.9</v>
       </c>
       <c r="D36">
         <f>MOD((C36+100),360)</f>
-        <v>296.3</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="E36">
         <v>100</v>
       </c>
       <c r="F36">
-        <v>94.1</v>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C37">
-        <v>195</v>
+        <v>196.3</v>
       </c>
       <c r="D37">
         <f>MOD((C37+100),360)</f>
-        <v>295</v>
-      </c>
-      <c r="E37" s="1">
-        <v>4.0999999999999996</v>
+        <v>296.3</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
       </c>
       <c r="F37">
-        <v>75.7</v>
+        <v>94.1</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="C38">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D38">
         <f>MOD((C38+100),360)</f>
-        <v>294</v>
-      </c>
-      <c r="E38">
-        <v>100</v>
+        <v>295</v>
+      </c>
+      <c r="E38" s="1">
+        <v>4.0999999999999996</v>
       </c>
       <c r="F38">
-        <v>96</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="C39">
         <v>194</v>
@@ -1958,193 +1973,193 @@
         <v>100</v>
       </c>
       <c r="F39">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40">
-        <v>9999</v>
+        <v>170</v>
+      </c>
+      <c r="B40" t="s">
+        <v>171</v>
       </c>
       <c r="C40">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D40">
         <f>MOD((C40+100),360)</f>
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="E40">
         <v>100</v>
       </c>
       <c r="F40">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41">
+        <v>9999</v>
+      </c>
+      <c r="C41">
         <v>180</v>
-      </c>
-      <c r="C41">
-        <v>165</v>
       </c>
       <c r="D41">
         <f>MOD((C41+100),360)</f>
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="E41">
         <v>100</v>
       </c>
       <c r="F41">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C42">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D42">
         <f>MOD((C42+100),360)</f>
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="E42">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F42">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C43">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="D43">
         <f>MOD((C43+100),360)</f>
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="E43">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="F43">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="C44">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D44">
         <f>MOD((C44+100),360)</f>
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="E44">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F44">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="C45">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D45">
         <f>MOD((C45+100),360)</f>
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="E45">
+        <v>193</v>
+      </c>
+      <c r="F45">
         <v>66</v>
-      </c>
-      <c r="F45">
-        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C46">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D46">
         <f>MOD((C46+100),360)</f>
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E46">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F46">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="C47">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <f>MOD((C47+100),360)</f>
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E47">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="F47">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C48">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D48">
         <f>MOD((C48+100),360)</f>
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E48">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="F48">
         <v>64</v>
@@ -2152,154 +2167,154 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C49">
-        <v>80.900000000000006</v>
+        <v>81</v>
       </c>
       <c r="D49">
         <f>MOD((C49+100),360)</f>
-        <v>180.9</v>
+        <v>181</v>
       </c>
       <c r="E49">
-        <v>86.3</v>
+        <v>100</v>
       </c>
       <c r="F49">
-        <v>71.8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C50">
-        <v>74.5</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D50">
         <f>MOD((C50+100),360)</f>
-        <v>174.5</v>
+        <v>180.9</v>
       </c>
       <c r="E50">
-        <v>71.2</v>
+        <v>86.3</v>
       </c>
       <c r="F50">
-        <v>77.599999999999994</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>38</v>
       </c>
       <c r="C51">
-        <v>51</v>
+        <v>74.5</v>
       </c>
       <c r="D51">
         <f>MOD((C51+100),360)</f>
-        <v>151</v>
+        <v>174.5</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>71.2</v>
       </c>
       <c r="F51">
-        <v>95</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="C52">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D52">
         <f>MOD((C52+100),360)</f>
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E52">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F52">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C53">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D53">
         <f>MOD((C53+100),360)</f>
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E53">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F53">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>163</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="C54">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D54">
         <f>MOD((C54+100),360)</f>
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E54">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F54">
-        <v>97</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="C55">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D55">
         <f>MOD((C55+100),360)</f>
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E55">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F55">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -2320,7 +2335,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
@@ -2341,10 +2356,10 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="C58">
         <v>36</v>
@@ -2354,7 +2369,7 @@
         <v>136</v>
       </c>
       <c r="E58">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F58">
         <v>100</v>
@@ -2362,20 +2377,20 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C59">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D59">
         <f>MOD((C59+100),360)</f>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E59">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F59">
         <v>100</v>
@@ -2383,10 +2398,10 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C60">
         <v>31</v>
@@ -2399,75 +2414,75 @@
         <v>100</v>
       </c>
       <c r="F60">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C61">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D61">
         <f>MOD((C61+100),360)</f>
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E61">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="F61">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C62">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D62">
         <f>MOD((C62+100),360)</f>
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E62">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F62">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="C63">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D63">
         <f>MOD((C63+100),360)</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E63">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F63">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="B64" t="s">
         <v>60</v>
@@ -2488,338 +2503,338 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D65">
         <f>MOD((C65+100),360)</f>
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E65">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="F65">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C66">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D66">
         <f>MOD((C66+100),360)</f>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E66">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="F66">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="C67">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D67">
         <f>MOD((C67+100),360)</f>
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E67">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F67">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D68">
         <f>MOD((C68+100),360)</f>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E68">
         <v>100</v>
       </c>
       <c r="F68">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C69">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D69">
         <f>MOD((C69+100),360)</f>
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E69">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F69">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>188</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>192</v>
       </c>
       <c r="C70">
-        <v>11.2</v>
+        <v>14</v>
       </c>
       <c r="D70">
         <f>MOD((C70+100),360)</f>
-        <v>111.2</v>
+        <v>114</v>
       </c>
       <c r="E70">
-        <v>84.7</v>
+        <v>78</v>
       </c>
       <c r="F70">
-        <v>92.2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="C71">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <f>MOD((C71+100),360)</f>
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E71">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F71">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="C72">
-        <v>8</v>
+        <v>11.2</v>
       </c>
       <c r="D72">
         <f>MOD((C72+100),360)</f>
-        <v>108</v>
+        <v>111.2</v>
       </c>
       <c r="E72">
-        <v>81</v>
+        <v>84.7</v>
       </c>
       <c r="F72">
-        <v>79</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C73">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D73">
         <f>MOD((C73+100),360)</f>
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E73">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="F73">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="C74">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <f>MOD((C74+100),360)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E74">
-        <v>74.2</v>
+        <v>81</v>
       </c>
       <c r="F74">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75">
         <v>7</v>
-      </c>
-      <c r="B75" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75">
-        <v>4</v>
       </c>
       <c r="D75">
         <f>MOD((C75+100),360)</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E75">
-        <v>92.5</v>
+        <v>76</v>
       </c>
       <c r="F75">
-        <v>89.4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D76">
         <f>MOD((C76+100),360)</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E76">
-        <v>97</v>
+        <v>74.2</v>
       </c>
       <c r="F76">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D77">
         <f>MOD((C77+100),360)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E77">
-        <v>78</v>
+        <v>92.5</v>
       </c>
       <c r="F77">
-        <v>80</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78">
         <f>MOD((C78+100),360)</f>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E78">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F78">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>168</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79">
         <f>MOD((C79+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E79">
         <v>90</v>
       </c>
       <c r="F79">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D80">
         <f>MOD((C80+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E80">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F80">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2845,10 +2860,10 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>62</v>
-      </c>
-      <c r="B82">
-        <v>666666</v>
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
+        <v>96</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2857,19 +2872,19 @@
         <f>MOD((C82+100),360)</f>
         <v>100</v>
       </c>
-      <c r="E82" s="1">
-        <v>0</v>
+      <c r="E82">
+        <v>93</v>
       </c>
       <c r="F82">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>54</v>
-      </c>
-      <c r="B83">
-        <v>444444</v>
+        <v>168</v>
+      </c>
+      <c r="B83" t="s">
+        <v>174</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2878,19 +2893,19 @@
         <f>MOD((C83+100),360)</f>
         <v>100</v>
       </c>
-      <c r="E83" s="1">
-        <v>0</v>
+      <c r="E83">
+        <v>90</v>
       </c>
       <c r="F83">
-        <v>27</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="B84">
-        <v>222222</v>
+        <v>666666</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2903,15 +2918,15 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>444444</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2924,15 +2939,15 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>222222</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2945,244 +2960,328 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" t="s">
-        <v>16</v>
+        <v>124</v>
+      </c>
+      <c r="B87">
+        <v>222222</v>
       </c>
       <c r="C87">
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="D87">
         <f>MOD((C87+100),360)</f>
-        <v>97.5</v>
-      </c>
-      <c r="E87">
-        <v>84.2</v>
+        <v>100</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>79.599999999999994</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>132</v>
-      </c>
-      <c r="B88" t="s">
-        <v>133</v>
+        <v>93</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <f>MOD((C88+100),360)</f>
-        <v>94</v>
-      </c>
-      <c r="E88">
-        <v>83</v>
+        <v>100</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>162</v>
-      </c>
-      <c r="B89" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <f>MOD((C89+100),360)</f>
-        <v>90</v>
-      </c>
-      <c r="E89">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>98</v>
-      </c>
-      <c r="B90" t="s">
-        <v>97</v>
+        <v>190</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>345</v>
+        <v>0</v>
       </c>
       <c r="D90">
         <f>MOD((C90+100),360)</f>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E90" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C91">
-        <v>336.8</v>
+        <v>357.5</v>
       </c>
       <c r="D91">
         <f>MOD((C91+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>97.5</v>
       </c>
       <c r="E91">
-        <v>67.5</v>
+        <v>84.2</v>
       </c>
       <c r="F91">
-        <v>91.8</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C92">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="D92">
         <f>MOD((C92+100),360)</f>
+        <v>94</v>
+      </c>
+      <c r="E92">
+        <v>83</v>
+      </c>
+      <c r="F92">
         <v>71</v>
-      </c>
-      <c r="E92">
-        <v>88</v>
-      </c>
-      <c r="F92">
-        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="B93" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="C93">
-        <v>328</v>
+        <v>350</v>
       </c>
       <c r="D93">
         <f>MOD((C93+100),360)</f>
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E93">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F93">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>166</v>
+        <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="C94">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="D94">
         <f>MOD((C94+100),360)</f>
-        <v>62</v>
-      </c>
-      <c r="E94">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="E94" s="1">
+        <v>11</v>
       </c>
       <c r="F94">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>181</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>182</v>
+        <v>20</v>
       </c>
       <c r="C95">
-        <v>308</v>
+        <v>336.8</v>
       </c>
       <c r="D95">
         <f>MOD((C95+100),360)</f>
-        <v>48</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="E95">
-        <v>69</v>
+        <v>67.5</v>
       </c>
       <c r="F95">
-        <v>47</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C96">
-        <v>288</v>
+        <v>331</v>
       </c>
       <c r="D96">
         <f>MOD((C96+100),360)</f>
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E96">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="F96">
-        <v>48</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B97" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C97">
-        <v>287.3</v>
+        <v>328</v>
       </c>
       <c r="D97">
         <f>MOD((C97+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E97">
+        <v>84</v>
+      </c>
+      <c r="F97">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>166</v>
+      </c>
+      <c r="B98" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98">
+        <v>322</v>
+      </c>
+      <c r="D98">
+        <f>MOD((C98+100),360)</f>
+        <v>62</v>
+      </c>
+      <c r="E98">
+        <v>100</v>
+      </c>
+      <c r="F98">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>181</v>
+      </c>
+      <c r="B99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99">
+        <v>308</v>
+      </c>
+      <c r="D99">
+        <f>MOD((C99+100),360)</f>
+        <v>48</v>
+      </c>
+      <c r="E99">
+        <v>69</v>
+      </c>
+      <c r="F99">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100">
+        <v>288</v>
+      </c>
+      <c r="D100">
+        <f>MOD((C100+100),360)</f>
+        <v>28</v>
+      </c>
+      <c r="E100">
+        <v>73</v>
+      </c>
+      <c r="F100">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>33</v>
+      </c>
+      <c r="B101" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101">
+        <v>287.3</v>
+      </c>
+      <c r="D101">
+        <f>MOD((C101+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E97">
+      <c r="E101">
         <v>81.3</v>
       </c>
-      <c r="F97">
+      <c r="F101">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F97">
-      <sortCondition descending="1" ref="D1:D97"/>
+    <sortState ref="A2:F101">
+      <sortCondition descending="1" ref="D1:D101"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added 16 new icons
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20580" yWindow="1540" windowWidth="12820" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="8120" windowWidth="30700" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="222">
   <si>
     <t>Twitter</t>
   </si>
@@ -601,6 +601,93 @@
   </si>
   <si>
     <t>E95C33</t>
+  </si>
+  <si>
+    <t>Codepen</t>
+  </si>
+  <si>
+    <t>Delicious</t>
+  </si>
+  <si>
+    <t>Designer News</t>
+  </si>
+  <si>
+    <t>DeviantART</t>
+  </si>
+  <si>
+    <t>Formspring</t>
+  </si>
+  <si>
+    <t>JSDB</t>
+  </si>
+  <si>
+    <t>jsFiddle</t>
+  </si>
+  <si>
+    <t>Layer Vault</t>
+  </si>
+  <si>
+    <t>Letterboxd</t>
+  </si>
+  <si>
+    <t>National Rail</t>
+  </si>
+  <si>
+    <t>Pingup</t>
+  </si>
+  <si>
+    <t>Proto.io</t>
+  </si>
+  <si>
+    <t>Rails</t>
+  </si>
+  <si>
+    <t>Trip Advisor</t>
+  </si>
+  <si>
+    <t>Typo3</t>
+  </si>
+  <si>
+    <t>Viadeo</t>
+  </si>
+  <si>
+    <t>F4982B</t>
+  </si>
+  <si>
+    <t>FF8700</t>
+  </si>
+  <si>
+    <t>A62C39</t>
+  </si>
+  <si>
+    <t>40C8F4</t>
+  </si>
+  <si>
+    <t>00B1AB</t>
+  </si>
+  <si>
+    <t>2C3641</t>
+  </si>
+  <si>
+    <t>26AE90</t>
+  </si>
+  <si>
+    <t>4679A4</t>
+  </si>
+  <si>
+    <t>DA320B</t>
+  </si>
+  <si>
+    <t>0076C0</t>
+  </si>
+  <si>
+    <t>4B5D50</t>
+  </si>
+  <si>
+    <t>1C52A2</t>
+  </si>
+  <si>
+    <t>3274D1</t>
   </si>
 </sst>
 </file>
@@ -632,7 +719,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,6 +729,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,7 +748,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -733,12 +826,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -777,6 +907,24 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -815,6 +963,24 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1144,11 +1310,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1285,10 +1451,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>217</v>
@@ -1298,18 +1464,18 @@
         <v>317</v>
       </c>
       <c r="E7">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="F7">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="C8">
         <v>217</v>
@@ -1319,1183 +1485,1183 @@
         <v>317</v>
       </c>
       <c r="E8">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F8">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>220</v>
       </c>
       <c r="C9">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D9">
         <f>MOD((C9+100),360)</f>
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E9">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F9">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="C10">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D10">
         <f>MOD((C10+100),360)</f>
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="F10">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C11">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D11">
         <f>MOD((C11+100),360)</f>
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F11">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="C12">
-        <v>210.4</v>
+        <v>213</v>
       </c>
       <c r="D12">
         <f>MOD((C12+100),360)</f>
-        <v>310.39999999999998</v>
+        <v>313</v>
       </c>
       <c r="E12">
-        <v>87.3</v>
+        <v>100</v>
       </c>
       <c r="F12">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>117</v>
       </c>
       <c r="C13">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D13">
         <f>MOD((C13+100),360)</f>
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E13">
-        <v>55.1</v>
+        <v>100</v>
       </c>
       <c r="F13">
-        <v>38.4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="C14">
-        <v>209.8</v>
+        <v>211</v>
       </c>
       <c r="D14">
         <f>MOD((C14+100),360)</f>
-        <v>309.8</v>
+        <v>311</v>
       </c>
       <c r="E14">
-        <v>66.8</v>
+        <v>32</v>
       </c>
       <c r="F14">
-        <v>76.900000000000006</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>176</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>208</v>
+        <v>210.4</v>
       </c>
       <c r="D15">
         <f>MOD((C15+100),360)</f>
-        <v>308</v>
+        <v>310.39999999999998</v>
       </c>
       <c r="E15">
-        <v>82</v>
+        <v>87.3</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
+        <v>202</v>
+      </c>
+      <c r="B16">
+        <v>3366</v>
       </c>
       <c r="C16">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D16">
         <f>MOD((C16+100),360)</f>
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E16">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F16">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D17">
         <f>MOD((C17+100),360)</f>
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E17">
-        <v>70</v>
+        <v>55.1</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>207</v>
+        <v>209.8</v>
       </c>
       <c r="D18">
         <f>MOD((C18+100),360)</f>
-        <v>307</v>
+        <v>309.8</v>
       </c>
       <c r="E18">
-        <v>59</v>
+        <v>66.8</v>
       </c>
       <c r="F18">
-        <v>61</v>
+        <v>76.900000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>176</v>
       </c>
       <c r="C19">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D19">
         <f>MOD((C19+100),360)</f>
-        <v>306</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5</v>
+        <v>308</v>
+      </c>
+      <c r="E19">
+        <v>82</v>
       </c>
       <c r="F19">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="C20">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D20">
         <f>MOD((C20+100),360)</f>
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F20">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="C21">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D21">
         <f>MOD((C21+100),360)</f>
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F21">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="C22">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D22">
         <f>MOD((C22+100),360)</f>
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E22">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="F22">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
       <c r="C23">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D23">
         <f>MOD((C23+100),360)</f>
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E23">
         <v>59</v>
       </c>
       <c r="F23">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>145</v>
+        <v>80</v>
       </c>
       <c r="C24">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>303</v>
-      </c>
-      <c r="E24">
-        <v>100</v>
+        <v>306</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="C25">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D25">
         <f>MOD((C25+100),360)</f>
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E25">
         <v>100</v>
       </c>
       <c r="F25">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="C26">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D26">
         <f>MOD((C26+100),360)</f>
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E26">
         <v>100</v>
       </c>
       <c r="F26">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="C27">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D27">
         <f>MOD((C27+100),360)</f>
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F27">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>175</v>
       </c>
       <c r="C28">
-        <v>201.8</v>
+        <v>204</v>
       </c>
       <c r="D28">
         <f>MOD((C28+100),360)</f>
-        <v>301.8</v>
+        <v>304</v>
       </c>
       <c r="E28">
-        <v>73.3</v>
+        <v>59</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="C29">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D29">
         <f>MOD((C29+100),360)</f>
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E29">
         <v>100</v>
       </c>
       <c r="F29">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="C30">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E30">
         <v>100</v>
       </c>
       <c r="F30">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="C31">
-        <v>199.8</v>
+        <v>203</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
-        <v>299.8</v>
+        <v>303</v>
       </c>
       <c r="E31">
-        <v>74.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="F31">
-        <v>87.8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="C32">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D32">
         <f>MOD((C32+100),360)</f>
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E32">
         <v>100</v>
       </c>
       <c r="F32">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="C33">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D33">
         <f>MOD((C33+100),360)</f>
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E33">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F33">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C34">
-        <v>198</v>
+        <v>201.8</v>
       </c>
       <c r="D34">
         <f>MOD((C34+100),360)</f>
-        <v>298</v>
+        <v>301.8</v>
       </c>
       <c r="E34">
-        <v>83</v>
+        <v>73.3</v>
       </c>
       <c r="F34">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C35">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D35">
         <f>MOD((C35+100),360)</f>
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
         <v>80</v>
-      </c>
-      <c r="F35">
-        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C36">
-        <v>196.9</v>
+        <v>200</v>
       </c>
       <c r="D36">
         <f>MOD((C36+100),360)</f>
-        <v>296.89999999999998</v>
+        <v>300</v>
       </c>
       <c r="E36">
         <v>100</v>
       </c>
       <c r="F36">
-        <v>69.400000000000006</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>196.3</v>
+        <v>199.8</v>
       </c>
       <c r="D37">
         <f>MOD((C37+100),360)</f>
-        <v>296.3</v>
+        <v>299.8</v>
       </c>
       <c r="E37">
-        <v>100</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="F37">
-        <v>94.1</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C38">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D38">
         <f>MOD((C38+100),360)</f>
-        <v>295</v>
-      </c>
-      <c r="E38" s="1">
-        <v>4.0999999999999996</v>
+        <v>299</v>
+      </c>
+      <c r="E38">
+        <v>79</v>
       </c>
       <c r="F38">
-        <v>75.7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="C39">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D39">
         <f>MOD((C39+100),360)</f>
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E39">
         <v>100</v>
       </c>
       <c r="F39">
-        <v>96</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>90</v>
       </c>
       <c r="C40">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D40">
         <f>MOD((C40+100),360)</f>
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E40">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F40">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41">
-        <v>9999</v>
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
       </c>
       <c r="C41">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="D41">
         <f>MOD((C41+100),360)</f>
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="E41">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F41">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="C42">
-        <v>165</v>
+        <v>196.9</v>
       </c>
       <c r="D42">
         <f>MOD((C42+100),360)</f>
-        <v>265</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="E42">
         <v>100</v>
       </c>
       <c r="F42">
-        <v>64</v>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="C43">
-        <v>149</v>
+        <v>196.3</v>
       </c>
       <c r="D43">
         <f>MOD((C43+100),360)</f>
-        <v>249</v>
+        <v>296.3</v>
       </c>
       <c r="E43">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F43">
-        <v>36</v>
+        <v>94.1</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="C44">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="D44">
         <f>MOD((C44+100),360)</f>
-        <v>232</v>
+        <v>295</v>
       </c>
       <c r="E44">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="F44">
-        <v>60</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C45">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="D45">
         <f>MOD((C45+100),360)</f>
-        <v>222</v>
-      </c>
-      <c r="E45">
-        <v>193</v>
+        <v>295</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.0999999999999996</v>
       </c>
       <c r="F45">
-        <v>66</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C46">
-        <v>88</v>
+        <v>194</v>
       </c>
       <c r="D46">
         <f>MOD((C46+100),360)</f>
-        <v>188</v>
+        <v>294</v>
       </c>
       <c r="E46">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="F46">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="C47">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="D47">
         <f>MOD((C47+100),360)</f>
-        <v>186</v>
+        <v>294</v>
       </c>
       <c r="E47">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="F47">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="B48">
+        <v>9999</v>
       </c>
       <c r="C48">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="D48">
         <f>MOD((C48+100),360)</f>
-        <v>184</v>
+        <v>280</v>
       </c>
       <c r="E48">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>203</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="C49">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="D49">
         <f>MOD((C49+100),360)</f>
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="E49">
         <v>100</v>
       </c>
       <c r="F49">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>215</v>
       </c>
       <c r="C50">
-        <v>80.900000000000006</v>
+        <v>167</v>
       </c>
       <c r="D50">
         <f>MOD((C50+100),360)</f>
-        <v>180.9</v>
+        <v>267</v>
       </c>
       <c r="E50">
-        <v>86.3</v>
+        <v>78</v>
       </c>
       <c r="F50">
-        <v>71.8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="C51">
-        <v>74.5</v>
+        <v>165</v>
       </c>
       <c r="D51">
         <f>MOD((C51+100),360)</f>
-        <v>174.5</v>
+        <v>265</v>
       </c>
       <c r="E51">
-        <v>71.2</v>
+        <v>100</v>
       </c>
       <c r="F51">
-        <v>77.599999999999994</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="C52">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="D52">
         <f>MOD((C52+100),360)</f>
-        <v>151</v>
+        <v>249</v>
       </c>
       <c r="E52">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F52">
-        <v>95</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>196</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>219</v>
       </c>
       <c r="C53">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="D53">
         <f>MOD((C53+100),360)</f>
-        <v>146</v>
+        <v>237</v>
       </c>
       <c r="E53">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="F53">
-        <v>100</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="C54">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D54">
         <f>MOD((C54+100),360)</f>
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="E54">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="F54">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>82</v>
       </c>
       <c r="C55">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D55">
         <f>MOD((C55+100),360)</f>
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="E55">
-        <v>79</v>
+        <v>193</v>
       </c>
       <c r="F55">
-        <v>97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" t="s">
-        <v>13</v>
+        <v>206</v>
+      </c>
+      <c r="B56">
+        <v>589442</v>
       </c>
       <c r="C56">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D56">
         <f>MOD((C56+100),360)</f>
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="E56">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="F56">
-        <v>100</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="C57">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="D57">
         <f>MOD((C57+100),360)</f>
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="E57">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="F57">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="C58">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="D58">
         <f>MOD((C58+100),360)</f>
-        <v>136</v>
+        <v>186</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="F58">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>53</v>
       </c>
       <c r="C59">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="D59">
         <f>MOD((C59+100),360)</f>
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="E59">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="F59">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C60">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="D60">
         <f>MOD((C60+100),360)</f>
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="E60">
         <v>100</v>
       </c>
       <c r="F60">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="C61">
-        <v>31</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D61">
         <f>MOD((C61+100),360)</f>
-        <v>131</v>
+        <v>180.9</v>
       </c>
       <c r="E61">
-        <v>100</v>
+        <v>86.3</v>
       </c>
       <c r="F61">
-        <v>96</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="C62">
-        <v>28</v>
+        <v>74.5</v>
       </c>
       <c r="D62">
         <f>MOD((C62+100),360)</f>
-        <v>128</v>
+        <v>174.5</v>
       </c>
       <c r="E62">
-        <v>66</v>
+        <v>71.2</v>
       </c>
       <c r="F62">
-        <v>78</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="C63">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D63">
         <f>MOD((C63+100),360)</f>
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="E63">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F63">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C64">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D64">
         <f>MOD((C64+100),360)</f>
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E64">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F64">
         <v>100</v>
@@ -2503,80 +2669,80 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C65">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D65">
         <f>MOD((C65+100),360)</f>
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="E65">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F65">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="C66">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D66">
         <f>MOD((C66+100),360)</f>
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="E66">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F66">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>13</v>
       </c>
       <c r="C67">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D67">
         <f>MOD((C67+100),360)</f>
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E67">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F67">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="C68">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D68">
         <f>MOD((C68+100),360)</f>
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="E68">
         <v>100</v>
@@ -2587,104 +2753,104 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="C69">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D69">
         <f>MOD((C69+100),360)</f>
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E69">
         <v>100</v>
       </c>
       <c r="F69">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="B70" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="C70">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D70">
         <f>MOD((C70+100),360)</f>
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="E70">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F70">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>110</v>
+        <v>208</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="C71">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D71">
         <f>MOD((C71+100),360)</f>
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E71">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F71">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>207</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="C72">
-        <v>11.2</v>
+        <v>32</v>
       </c>
       <c r="D72">
         <f>MOD((C72+100),360)</f>
-        <v>111.2</v>
+        <v>132</v>
       </c>
       <c r="E72">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F72">
-        <v>92.2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="B73" t="s">
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="C73">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D73">
         <f>MOD((C73+100),360)</f>
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="E73">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F73">
         <v>100</v>
@@ -2692,596 +2858,932 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D74">
         <f>MOD((C74+100),360)</f>
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="E74">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F74">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
       <c r="C75">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D75">
         <f>MOD((C75+100),360)</f>
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="E75">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F75">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C76">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D76">
         <f>MOD((C76+100),360)</f>
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="E76">
-        <v>74.2</v>
+        <v>87</v>
       </c>
       <c r="F76">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D77">
         <f>MOD((C77+100),360)</f>
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="E77">
-        <v>92.5</v>
+        <v>100</v>
       </c>
       <c r="F77">
-        <v>89.4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D78">
         <f>MOD((C78+100),360)</f>
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="E78">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F78">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D79">
         <f>MOD((C79+100),360)</f>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="E79">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="F79">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D80">
         <f>MOD((C80+100),360)</f>
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E80">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F80">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81">
-        <v>870000</v>
+        <v>120</v>
+      </c>
+      <c r="B81" t="s">
+        <v>121</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D81">
         <f>MOD((C81+100),360)</f>
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E81">
         <v>100</v>
       </c>
       <c r="F81">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D82">
         <f>MOD((C82+100),360)</f>
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E82">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F82">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B83" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D83">
         <f>MOD((C83+100),360)</f>
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E83">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F83">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84">
-        <v>666666</v>
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
+        <v>111</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D84">
         <f>MOD((C84+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E84" s="1">
-        <v>0</v>
+        <v>112</v>
+      </c>
+      <c r="E84">
+        <v>84</v>
       </c>
       <c r="F84">
-        <v>40</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>54</v>
-      </c>
-      <c r="B85">
-        <v>444444</v>
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>11.2</v>
       </c>
       <c r="D85">
         <f>MOD((C85+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E85" s="1">
-        <v>0</v>
+        <v>111.2</v>
+      </c>
+      <c r="E85">
+        <v>84.7</v>
       </c>
       <c r="F85">
-        <v>27</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>191</v>
-      </c>
-      <c r="B86">
-        <v>222222</v>
+        <v>198</v>
+      </c>
+      <c r="B86" t="s">
+        <v>217</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D86">
         <f>MOD((C86+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E86" s="1">
-        <v>0</v>
+        <v>111</v>
+      </c>
+      <c r="E86">
+        <v>95</v>
       </c>
       <c r="F86">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>124</v>
-      </c>
-      <c r="B87">
-        <v>222222</v>
+        <v>184</v>
+      </c>
+      <c r="B87" t="s">
+        <v>185</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D87">
         <f>MOD((C87+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E87" s="1">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="E87">
+        <v>98</v>
       </c>
       <c r="F87">
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>93</v>
-      </c>
-      <c r="B88">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="B88" t="s">
+        <v>123</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D88">
         <f>MOD((C88+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E88" s="1">
-        <v>0</v>
+        <v>108</v>
+      </c>
+      <c r="E88">
+        <v>81</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>167</v>
-      </c>
-      <c r="B89">
-        <v>0</v>
+        <v>186</v>
+      </c>
+      <c r="B89" t="s">
+        <v>187</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D89">
         <f>MOD((C89+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E89" s="1">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="E89">
+        <v>76</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>190</v>
-      </c>
-      <c r="B90">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="B90" t="s">
+        <v>42</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D90">
         <f>MOD((C90+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E90" s="1">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="E90">
+        <v>74.2</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C91">
-        <v>357.5</v>
+        <v>4</v>
       </c>
       <c r="D91">
         <f>MOD((C91+100),360)</f>
-        <v>97.5</v>
+        <v>104</v>
       </c>
       <c r="E91">
-        <v>84.2</v>
+        <v>92.5</v>
       </c>
       <c r="F91">
-        <v>79.599999999999994</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="C92">
-        <v>354</v>
+        <v>3</v>
       </c>
       <c r="D92">
         <f>MOD((C92+100),360)</f>
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E92">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="F92">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>162</v>
+        <v>70</v>
       </c>
       <c r="B93" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="C93">
-        <v>350</v>
+        <v>2</v>
       </c>
       <c r="D93">
         <f>MOD((C93+100),360)</f>
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E93">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F93">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C94">
-        <v>345</v>
+        <v>2</v>
       </c>
       <c r="D94">
         <f>MOD((C94+100),360)</f>
-        <v>85</v>
-      </c>
-      <c r="E94" s="1">
-        <v>11</v>
+        <v>102</v>
+      </c>
+      <c r="E94">
+        <v>90</v>
       </c>
       <c r="F94">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>174</v>
       </c>
       <c r="C95">
-        <v>336.8</v>
+        <v>0</v>
       </c>
       <c r="D95">
         <f>MOD((C95+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>100</v>
       </c>
       <c r="E95">
-        <v>67.5</v>
+        <v>90</v>
       </c>
       <c r="F95">
-        <v>91.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="C96">
-        <v>331</v>
+        <v>0</v>
       </c>
       <c r="D96">
         <f>MOD((C96+100),360)</f>
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E96">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F96">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>67</v>
-      </c>
-      <c r="B97" t="s">
-        <v>71</v>
+        <v>125</v>
+      </c>
+      <c r="B97">
+        <v>870000</v>
       </c>
       <c r="C97">
-        <v>328</v>
+        <v>0</v>
       </c>
       <c r="D97">
         <f>MOD((C97+100),360)</f>
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E97">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F97">
-        <v>93</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>166</v>
-      </c>
-      <c r="B98" t="s">
-        <v>172</v>
+        <v>62</v>
+      </c>
+      <c r="B98">
+        <v>666666</v>
       </c>
       <c r="C98">
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="D98">
         <f>MOD((C98+100),360)</f>
-        <v>62</v>
-      </c>
-      <c r="E98">
-        <v>100</v>
+        <v>100</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>181</v>
-      </c>
-      <c r="B99" t="s">
-        <v>182</v>
+        <v>54</v>
+      </c>
+      <c r="B99">
+        <v>444444</v>
       </c>
       <c r="C99">
-        <v>308</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <f>MOD((C99+100),360)</f>
-        <v>48</v>
-      </c>
-      <c r="E99">
-        <v>69</v>
+        <v>100</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>105</v>
-      </c>
-      <c r="B100" t="s">
-        <v>108</v>
+        <v>191</v>
+      </c>
+      <c r="B100">
+        <v>222222</v>
       </c>
       <c r="C100">
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="D100">
         <f>MOD((C100+100),360)</f>
-        <v>28</v>
-      </c>
-      <c r="E100">
-        <v>73</v>
+        <v>100</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>33</v>
-      </c>
-      <c r="B101" t="s">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="B101">
+        <v>222222</v>
       </c>
       <c r="C101">
-        <v>287.3</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <f>MOD((C101+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <f>MOD((C102+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>167</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <f>MOD((C103+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <f>MOD((C104+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105">
+        <v>357.5</v>
+      </c>
+      <c r="D105">
+        <f>MOD((C105+100),360)</f>
+        <v>97.5</v>
+      </c>
+      <c r="E105">
+        <v>84.2</v>
+      </c>
+      <c r="F105">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>132</v>
+      </c>
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="C106">
+        <v>354</v>
+      </c>
+      <c r="D106">
+        <f>MOD((C106+100),360)</f>
+        <v>94</v>
+      </c>
+      <c r="E106">
+        <v>83</v>
+      </c>
+      <c r="F106">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" t="s">
+        <v>211</v>
+      </c>
+      <c r="C107">
+        <v>354</v>
+      </c>
+      <c r="D107">
+        <f>MOD((C107+100),360)</f>
+        <v>94</v>
+      </c>
+      <c r="E107">
+        <v>73</v>
+      </c>
+      <c r="F107">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>162</v>
+      </c>
+      <c r="B108" t="s">
+        <v>173</v>
+      </c>
+      <c r="C108">
+        <v>350</v>
+      </c>
+      <c r="D108">
+        <f>MOD((C108+100),360)</f>
+        <v>90</v>
+      </c>
+      <c r="E108">
+        <v>91</v>
+      </c>
+      <c r="F108">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>193</v>
+      </c>
+      <c r="B109" t="s">
+        <v>97</v>
+      </c>
+      <c r="C109">
+        <v>345</v>
+      </c>
+      <c r="D109">
+        <f>MOD((C109+100),360)</f>
+        <v>85</v>
+      </c>
+      <c r="E109" s="2">
+        <v>11</v>
+      </c>
+      <c r="F109">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>98</v>
+      </c>
+      <c r="B110" t="s">
+        <v>97</v>
+      </c>
+      <c r="C110">
+        <v>345</v>
+      </c>
+      <c r="D110">
+        <f>MOD((C110+100),360)</f>
+        <v>85</v>
+      </c>
+      <c r="E110" s="1">
+        <v>11</v>
+      </c>
+      <c r="F110">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111">
+        <v>336.8</v>
+      </c>
+      <c r="D111">
+        <f>MOD((C111+100),360)</f>
+        <v>76.800000000000011</v>
+      </c>
+      <c r="E111">
+        <v>67.5</v>
+      </c>
+      <c r="F111">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>152</v>
+      </c>
+      <c r="B112" t="s">
+        <v>158</v>
+      </c>
+      <c r="C112">
+        <v>331</v>
+      </c>
+      <c r="D112">
+        <f>MOD((C112+100),360)</f>
+        <v>71</v>
+      </c>
+      <c r="E112">
+        <v>88</v>
+      </c>
+      <c r="F112">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>67</v>
+      </c>
+      <c r="B113" t="s">
+        <v>71</v>
+      </c>
+      <c r="C113">
+        <v>328</v>
+      </c>
+      <c r="D113">
+        <f>MOD((C113+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E113">
+        <v>84</v>
+      </c>
+      <c r="F113">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>166</v>
+      </c>
+      <c r="B114" t="s">
+        <v>172</v>
+      </c>
+      <c r="C114">
+        <v>322</v>
+      </c>
+      <c r="D114">
+        <f>MOD((C114+100),360)</f>
+        <v>62</v>
+      </c>
+      <c r="E114">
+        <v>100</v>
+      </c>
+      <c r="F114">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>181</v>
+      </c>
+      <c r="B115" t="s">
+        <v>182</v>
+      </c>
+      <c r="C115">
+        <v>308</v>
+      </c>
+      <c r="D115">
+        <f>MOD((C115+100),360)</f>
+        <v>48</v>
+      </c>
+      <c r="E115">
+        <v>69</v>
+      </c>
+      <c r="F115">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116" t="s">
+        <v>108</v>
+      </c>
+      <c r="C116">
+        <v>288</v>
+      </c>
+      <c r="D116">
+        <f>MOD((C116+100),360)</f>
+        <v>28</v>
+      </c>
+      <c r="E116">
+        <v>73</v>
+      </c>
+      <c r="F116">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" t="s">
+        <v>33</v>
+      </c>
+      <c r="B117" t="s">
+        <v>34</v>
+      </c>
+      <c r="C117">
+        <v>287.3</v>
+      </c>
+      <c r="D117">
+        <f>MOD((C117+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E101">
+      <c r="E117">
         <v>81.3</v>
       </c>
-      <c r="F101">
+      <c r="F117">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F101">
-      <sortCondition descending="1" ref="D1:D101"/>
+    <sortState ref="A2:F117">
+      <sortCondition descending="1" ref="D1:D117"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>